<commit_message>
INCLUIDO COD DO EVENTO
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\Efetuar_Evento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06D29802-5CF7-4E26-8809-7383086A081C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF399FD5-6561-4B5B-855F-32F2C8B0D577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FA54B1B-2027-4D38-972F-9E68F25CE597}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -286,26 +283,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Plan4"/>
-      <sheetName val="RELATORIO PBI"/>
-      <sheetName val="REGRA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -608,7 +585,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,9 +630,8 @@
       <c r="B2" s="7">
         <v>45505</v>
       </c>
-      <c r="C2" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C2" s="8">
+        <v>27</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>10</v>
@@ -682,9 +658,8 @@
       <c r="B3" s="7">
         <v>45505</v>
       </c>
-      <c r="C3" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C3" s="8">
+        <v>27</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>12</v>
@@ -711,9 +686,8 @@
       <c r="B4" s="7">
         <v>45505</v>
       </c>
-      <c r="C4" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C4" s="8">
+        <v>27</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>13</v>
@@ -740,9 +714,8 @@
       <c r="B5" s="7">
         <v>45505</v>
       </c>
-      <c r="C5" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C5" s="8">
+        <v>27</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>14</v>
@@ -769,9 +742,8 @@
       <c r="B6" s="7">
         <v>45506</v>
       </c>
-      <c r="C6" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C6" s="8">
+        <v>27</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>15</v>
@@ -798,9 +770,8 @@
       <c r="B7" s="7">
         <v>45498</v>
       </c>
-      <c r="C7" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C7" s="8">
+        <v>27</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>16</v>
@@ -827,9 +798,8 @@
       <c r="B8" s="7">
         <v>45503</v>
       </c>
-      <c r="C8" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C8" s="8">
+        <v>27</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>16</v>
@@ -856,9 +826,8 @@
       <c r="B9" s="7">
         <v>45504</v>
       </c>
-      <c r="C9" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C9" s="8">
+        <v>27</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>16</v>
@@ -885,9 +854,8 @@
       <c r="B10" s="7">
         <v>45504</v>
       </c>
-      <c r="C10" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C10" s="8">
+        <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>18</v>
@@ -914,9 +882,8 @@
       <c r="B11" s="7">
         <v>45505</v>
       </c>
-      <c r="C11" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C11" s="8">
+        <v>27</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>19</v>
@@ -943,9 +910,8 @@
       <c r="B12" s="7">
         <v>45507</v>
       </c>
-      <c r="C12" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C12" s="8">
+        <v>27</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>20</v>
@@ -972,9 +938,8 @@
       <c r="B13" s="7">
         <v>45503</v>
       </c>
-      <c r="C13" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C13" s="8">
+        <v>27</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>21</v>
@@ -1001,9 +966,8 @@
       <c r="B14" s="7">
         <v>45503</v>
       </c>
-      <c r="C14" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C14" s="8">
+        <v>27</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>21</v>
@@ -1030,9 +994,8 @@
       <c r="B15" s="7">
         <v>45503</v>
       </c>
-      <c r="C15" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C15" s="8">
+        <v>27</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>21</v>
@@ -1059,9 +1022,8 @@
       <c r="B16" s="7">
         <v>45503</v>
       </c>
-      <c r="C16" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C16" s="8">
+        <v>27</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>21</v>
@@ -1088,9 +1050,8 @@
       <c r="B17" s="7">
         <v>45503</v>
       </c>
-      <c r="C17" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C17" s="8">
+        <v>27</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>23</v>
@@ -1117,9 +1078,8 @@
       <c r="B18" s="7">
         <v>45503</v>
       </c>
-      <c r="C18" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C18" s="8">
+        <v>20</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>24</v>
@@ -1146,9 +1106,8 @@
       <c r="B19" s="7">
         <v>45506</v>
       </c>
-      <c r="C19" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C19" s="8">
+        <v>27</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>26</v>
@@ -1175,9 +1134,8 @@
       <c r="B20" s="7">
         <v>45503</v>
       </c>
-      <c r="C20" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C20" s="8">
+        <v>27</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>27</v>
@@ -1204,9 +1162,8 @@
       <c r="B21" s="7">
         <v>45503</v>
       </c>
-      <c r="C21" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C21" s="8">
+        <v>27</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>28</v>
@@ -1233,9 +1190,8 @@
       <c r="B22" s="7">
         <v>45505</v>
       </c>
-      <c r="C22" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C22" s="8">
+        <v>27</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>21</v>
@@ -1262,9 +1218,8 @@
       <c r="B23" s="7">
         <v>45503</v>
       </c>
-      <c r="C23" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C23" s="8">
+        <v>27</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>28</v>
@@ -1291,9 +1246,8 @@
       <c r="B24" s="7">
         <v>45503</v>
       </c>
-      <c r="C24" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C24" s="8">
+        <v>27</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>28</v>
@@ -1320,9 +1274,8 @@
       <c r="B25" s="7">
         <v>45505</v>
       </c>
-      <c r="C25" s="8" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C25" s="8">
+        <v>27</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>21</v>
@@ -1349,9 +1302,8 @@
       <c r="B26" s="13">
         <v>45503</v>
       </c>
-      <c r="C26" s="14" t="str">
-        <f>IFERROR(VLOOKUP([1]!Tabela2[[#This Row],[TIPO EVENTO]],[1]REGRA!#REF!,2,0),"")</f>
-        <v/>
+      <c r="C26" s="14">
+        <v>27</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
teste 3 finalizado com sucesso
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -1,99 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\Efetuar_Evento\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8817C3-5CE0-4602-9691-1016B8384299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t>EVENTO</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>PLACA</t>
-  </si>
-  <si>
-    <t>VALOR</t>
-  </si>
-  <si>
-    <t>OBSERVAÇÃO</t>
-  </si>
-  <si>
-    <t>FILIAL</t>
-  </si>
-  <si>
-    <t>SERIE</t>
-  </si>
-  <si>
-    <t>MANIFESTO</t>
-  </si>
-  <si>
-    <t>MOTIVO</t>
-  </si>
-  <si>
-    <t>EPS3I64</t>
-  </si>
-  <si>
-    <t>REEMBOLSO DE PEDAGIO</t>
-  </si>
-  <si>
-    <t>APS-4127</t>
-  </si>
-  <si>
-    <t>EZU9C84</t>
-  </si>
-  <si>
-    <t>REEMBOLSO DE PEDÁGIO</t>
-  </si>
-  <si>
-    <t>DVT7940</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -112,7 +54,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,58 +127,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -536,187 +537,248 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>EVENTO</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>DATA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>PLACA</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>VALOR</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>OBSERVAÇÃO</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>FILIAL</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>SERIE</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>MANIFESTO</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>MOTIVO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="n">
+        <v>1549304</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>45503</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>APS-4127</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>REEMBOLSO DE PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="I2" s="7" t="n">
+        <v>214065</v>
+      </c>
+      <c r="J2" s="10" t="n"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="6">
+    <row r="3">
+      <c r="A3" s="9" t="n">
+        <v>1549305</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>45505</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>27</v>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>EPS3I64</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>REEMBOLSO DE PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>214054</v>
+      </c>
+      <c r="J3" s="10" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="n">
+        <v>1549306</v>
+      </c>
+      <c r="B4" s="12" t="n">
         <v>45503</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C4" s="13" t="n">
         <v>27</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="D4" s="13" t="inlineStr">
+        <is>
+          <t>APS-4127</t>
+        </is>
+      </c>
+      <c r="E4" s="14" t="n">
         <v>22.8</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="F4" s="11" t="inlineStr">
+        <is>
+          <t>REEMBOLSO DE PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H4" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="7">
-        <v>214065</v>
-      </c>
-      <c r="J2" s="10"/>
+      <c r="I4" s="13" t="n">
+        <v>214226</v>
+      </c>
+      <c r="J4" s="15" t="n"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6">
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1549307</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>45505</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C5" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8">
-        <v>58.3</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>EZU9C84</t>
+        </is>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>REEMBOLSO DE PEDÁGIO</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="7">
-        <v>214054</v>
-      </c>
-      <c r="J3" s="10"/>
+      <c r="I5" s="7" t="n">
+        <v>214992</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12">
-        <v>45503</v>
-      </c>
-      <c r="C4" s="13">
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1549308</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>45506</v>
+      </c>
+      <c r="C6" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="14">
-        <v>22.8</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="13">
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>DVT7940</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>384.6</v>
+      </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>REEMBOLSO DE PEDÁGIO</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H6" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="13">
-        <v>214226</v>
-      </c>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>45505</v>
-      </c>
-      <c r="C5" s="7">
-        <v>27</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="8">
-        <v>27.9</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7">
-        <v>214992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>45506</v>
-      </c>
-      <c r="C6" s="7">
-        <v>27</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="8">
-        <v>384.6</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="I6" s="7" t="n">
         <v>215043</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ERRO DE RATEIO DO EVENTO</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizado evento no pc escritorio dia 08.08
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -102,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -122,6 +122,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,16 +500,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="42.28515625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="40" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -565,25 +567,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1550086</v>
+        <v>1551626</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="C2" t="n">
         <v>27</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DHY4D23</t>
+          <t>GET2050</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>39.8</v>
+        <v>189.4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>REEMBOLSO PEDAGIO</t>
+          <t>REEMBOLSO DE PEDÁGIO</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -593,30 +595,30 @@
         <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>214914</v>
+        <v>215363</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1550092</v>
+        <v>1551631</v>
       </c>
       <c r="B3" s="6" t="n">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="C3" t="n">
         <v>27</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>FJI7F48</t>
+          <t>EFO9188</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>23.8</v>
+        <v>305.9</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>REEMBOLSO PEDAGIO</t>
+          <t>REEMBOLSO DE PEDÁGIO</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -626,30 +628,30 @@
         <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>215001</v>
+        <v>215365</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1550093</v>
+        <v>1551636</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>45505</v>
+        <v>45510</v>
       </c>
       <c r="C4" t="n">
         <v>27</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>FVZ8J15</t>
+          <t>HAN7E35</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>58.7</v>
+        <v>145</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>REEMBOLSO PEDAGIO</t>
+          <t>REEMBOLSO DE PEDÁGIO</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -659,26 +661,26 @@
         <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>214913</v>
+        <v>215366</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1550094</v>
+        <v>1551641</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>45507</v>
+        <v>45510</v>
       </c>
       <c r="C5" t="n">
         <v>27</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CUK3D79</t>
+          <t>DJB7A66</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>19.2</v>
+        <v>298.05</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -692,26 +694,26 @@
         <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>215148</v>
+        <v>215367</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1550095</v>
+        <v>1551647</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>45507</v>
+        <v>45510</v>
       </c>
       <c r="C6" t="n">
         <v>27</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DVT7940</t>
+          <t>DTE2J80</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>527.6</v>
+        <v>227.16</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -725,26 +727,26 @@
         <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>215149</v>
+        <v>215368</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1550096</v>
+        <v>1551653</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>45507</v>
+        <v>45510</v>
       </c>
       <c r="C7" t="n">
         <v>27</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DJB7A66</t>
+          <t>FCC0E56</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>15</v>
+        <v>160.8</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -758,26 +760,26 @@
         <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>215150</v>
+        <v>215369</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1550097</v>
+        <v>1551658</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>45507</v>
+        <v>45510</v>
       </c>
       <c r="C8" t="n">
         <v>27</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>FCC0E56</t>
+          <t>BWR2I48</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>19.2</v>
+        <v>163.4</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -791,152 +793,8 @@
         <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>215154</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1550098</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>45509</v>
-      </c>
-      <c r="C9" t="n">
-        <v>27</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>EZU9C84</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>27.9</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" t="n">
-        <v>215188</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="6" t="n"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="6" t="n"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="6" t="n"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="6" t="n"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="6" t="n"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="6" t="n"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="6" t="n"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="6" t="n"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="6" t="n"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="6" t="n"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="6" t="n"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="6" t="n"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="6" t="n"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="6" t="n"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="6" t="n"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="6" t="n"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="6" t="n"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="6" t="n"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="6" t="n"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="6" t="n"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="6" t="n"/>
-    </row>
-    <row r="31">
-      <c r="B31" s="6" t="n"/>
-    </row>
-    <row r="32">
-      <c r="B32" s="6" t="n"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="6" t="n"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="6" t="n"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="6" t="n"/>
-    </row>
-    <row r="36">
-      <c r="B36" s="6" t="n"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="6" t="n"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="6" t="n"/>
-    </row>
-    <row r="39">
-      <c r="B39" s="6" t="n"/>
-    </row>
-    <row r="40">
-      <c r="B40" s="6" t="n"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="6" t="n"/>
-    </row>
-    <row r="42">
-      <c r="B42" s="6" t="n"/>
-    </row>
-    <row r="43">
-      <c r="B43" s="6" t="n"/>
-    </row>
-    <row r="44">
-      <c r="B44" s="6" t="n"/>
-    </row>
-    <row r="45">
-      <c r="B45" s="6" t="n"/>
-    </row>
-    <row r="46">
-      <c r="B46" s="6" t="n"/>
+        <v>215371</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>

</xml_diff>

<commit_message>
incluido entrar na tela de evento
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -102,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -122,7 +122,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,14 +502,14 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
+      <selection activeCell="B3" sqref="B3:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.7109375" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="40" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="11.5703125" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="40" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -567,7 +566,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1551626</v>
+        <v>1553046</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>45510</v>
@@ -599,202 +598,22 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1551631</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>45510</v>
-      </c>
-      <c r="C3" t="n">
-        <v>27</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>EFO9188</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>305.9</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>215365</v>
-      </c>
+      <c r="B3" s="6" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1551636</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>45510</v>
-      </c>
-      <c r="C4" t="n">
-        <v>27</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>HAN7E35</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>145</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" t="n">
-        <v>215366</v>
-      </c>
+      <c r="B4" s="6" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1551641</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>45510</v>
-      </c>
-      <c r="C5" t="n">
-        <v>27</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>DJB7A66</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>298.05</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>215367</v>
-      </c>
+      <c r="B5" s="6" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1551647</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>45510</v>
-      </c>
-      <c r="C6" t="n">
-        <v>27</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>DTE2J80</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>227.16</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" t="n">
-        <v>215368</v>
-      </c>
+      <c r="B6" s="6" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1551653</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>45510</v>
-      </c>
-      <c r="C7" t="n">
-        <v>27</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>FCC0E56</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>160.8</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>215369</v>
-      </c>
+      <c r="B7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1551658</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>45510</v>
-      </c>
-      <c r="C8" t="n">
-        <v>27</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>BWR2I48</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>163.4</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" t="n">
-        <v>215371</v>
-      </c>
+      <c r="B8" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>

</xml_diff>

<commit_message>
rodado dia 12.08 e feito melhorias de avisos de erro
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2340" yWindow="2340" windowWidth="19170" windowHeight="11400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -59,7 +59,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -98,11 +98,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -120,6 +131,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -502,12 +516,13 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I8"/>
+      <selection activeCell="A12" sqref="A2:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.140625" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="40" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="11.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
@@ -566,25 +581,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1553046</v>
+        <v>1553576</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>45510</v>
+        <v>45511</v>
       </c>
       <c r="C2" t="n">
         <v>27</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GET2050</t>
+          <t>LYY8583</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>189.4</v>
+        <v>138.9</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>REEMBOLSO DE PEDÁGIO</t>
+          <t>REEMBOLSO PEDAGIO</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -594,26 +609,206 @@
         <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>215363</v>
+        <v>215415</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
+      <c r="A3" t="n">
+        <v>1553577</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>45509</v>
+      </c>
+      <c r="C3" t="n">
+        <v>27</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>DMD2D08</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>40.2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>REEMBOLSO PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>215250</v>
+      </c>
     </row>
     <row r="4">
-      <c r="B4" s="6" t="n"/>
+      <c r="A4" t="n">
+        <v>1553580</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>45511</v>
+      </c>
+      <c r="C4" t="n">
+        <v>27</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>DMD2D08</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>REEMBOLSO PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>215421</v>
+      </c>
     </row>
     <row r="5">
-      <c r="B5" s="6" t="n"/>
+      <c r="A5" t="n">
+        <v>1553581</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>45512</v>
+      </c>
+      <c r="C5" t="n">
+        <v>27</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>DMD2D08</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>REEMBOLSO PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>215632</v>
+      </c>
     </row>
     <row r="6">
-      <c r="B6" s="6" t="n"/>
+      <c r="A6" t="n">
+        <v>1553582</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>45512</v>
+      </c>
+      <c r="C6" t="n">
+        <v>27</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>EGM9B58</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>REEMBOLSO PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>215529</v>
+      </c>
     </row>
     <row r="7">
-      <c r="B7" s="6" t="n"/>
+      <c r="A7" t="n">
+        <v>1553583</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>45511</v>
+      </c>
+      <c r="C7" t="n">
+        <v>27</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>DBB6021</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>67.8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>REEMBOLSO PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>215399</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="6" t="n"/>
+      <c r="A8" t="n">
+        <v>1553584</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>45511</v>
+      </c>
+      <c r="C8" t="n">
+        <v>27</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>HJF*0J75</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>REEMBOLSO PEDAGIO</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>215509</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>

</xml_diff>

<commit_message>
feito teste no pc da suely
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -9,14 +9,14 @@
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,6 +29,13 @@
       <family val="2"/>
       <b val="1"/>
       <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -59,7 +66,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,17 +105,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -130,12 +126,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,18 +507,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A2:XFD12"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10.140625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="40" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="11.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="10.140625" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="40" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -581,25 +575,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1553576</v>
+        <v>1557598</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>45511</v>
+        <v>45516</v>
       </c>
       <c r="C2" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>LYY8583</t>
+          <t>NTN&amp;2311</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>138.9</v>
+        <v>550</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>REEMBOLSO PEDAGIO</t>
+          <t>ROTA ITINERANTE DE 2 DIAS</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -609,205 +603,7 @@
         <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>215415</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1553577</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>45509</v>
-      </c>
-      <c r="C3" t="n">
-        <v>27</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>DMD2D08</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>40.2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>REEMBOLSO PEDAGIO</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>215250</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1553580</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>45511</v>
-      </c>
-      <c r="C4" t="n">
-        <v>27</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>DMD2D08</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>22.8</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>REEMBOLSO PEDAGIO</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" t="n">
-        <v>215421</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1553581</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>45512</v>
-      </c>
-      <c r="C5" t="n">
-        <v>27</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>DMD2D08</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>45.2</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>REEMBOLSO PEDAGIO</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>215632</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1553582</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>45512</v>
-      </c>
-      <c r="C6" t="n">
-        <v>27</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>EGM9B58</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>29.2</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>REEMBOLSO PEDAGIO</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" t="n">
-        <v>215529</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1553583</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>45511</v>
-      </c>
-      <c r="C7" t="n">
-        <v>27</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>DBB6021</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>67.8</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>REEMBOLSO PEDAGIO</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>215399</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1553584</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>45511</v>
-      </c>
-      <c r="C8" t="n">
-        <v>27</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>HJF*0J75</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>69.40000000000001</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>REEMBOLSO PEDAGIO</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" t="n">
-        <v>215509</v>
+        <v>215874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustado para rodar no not suely
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -1,48 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jetta\Documents\Efetuar_Evento\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2340" yWindow="2340" windowWidth="19170" windowHeight="11400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="19170" windowHeight="11400"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+  <si>
+    <t>EVENTO</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>PLACA</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>OBSERVAÇÃO</t>
+  </si>
+  <si>
+    <t>FILIAL</t>
+  </si>
+  <si>
+    <t>SERIE</t>
+  </si>
+  <si>
+    <t>MANIFESTO</t>
+  </si>
+  <si>
+    <t>MOTIVO</t>
+  </si>
+  <si>
+    <t>ESU-5H70</t>
+  </si>
+  <si>
+    <t>REEMBOLSO DE PEDAGIO</t>
+  </si>
+  <si>
+    <t>DOCUMENTO NAO ENCONTRADO</t>
+  </si>
+  <si>
+    <t>GAU8A61</t>
+  </si>
+  <si>
+    <t>KXC3H55</t>
+  </si>
+  <si>
+    <t>PWM6547</t>
+  </si>
+  <si>
+    <t>EAX3641</t>
+  </si>
+  <si>
+    <t>MOTORISTA NAO ENCONTRADO</t>
+  </si>
+  <si>
+    <t>FEJ8959</t>
+  </si>
+  <si>
+    <t>MHP0N26</t>
+  </si>
+  <si>
+    <t>VEICULO NAO ENCONTRADO OU INATIVO</t>
+  </si>
+  <si>
+    <t>EWJ1210</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -61,7 +137,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,100 +185,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -502,111 +520,636 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="10.7109375" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="10.140625" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
-    <col width="40" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="11.5703125" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
+    <col min="2" max="2" width="10.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>EVENTO</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>DATA</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>COD</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>PLACA</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>VALOR</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>OBSERVAÇÃO</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>FILIAL</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>SERIE</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>MANIFESTO</t>
-        </is>
-      </c>
-      <c r="J1" s="5" t="inlineStr">
-        <is>
-          <t>MOTIVO</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1557598</v>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>45516</v>
-      </c>
-      <c r="C2" t="n">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1559341</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45517</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>122.42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>215905</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="7"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="7"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="7"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="7"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="7"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="7"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="7"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="7"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="7"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="7"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="7"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="7"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="7"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="7"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="7"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="7"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="7"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="7"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="7"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="7"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="7"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="7"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="7"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="7"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="7"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="7"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="7"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="7"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="7"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="7"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="7"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="7"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="7"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1559103</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45519</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>76.2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <v>24364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1559106</v>
+      </c>
+      <c r="B3" s="6">
+        <v>45519</v>
+      </c>
+      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>22.8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>24369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1559107</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45519</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>10.3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>24362</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>45519</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>3.2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>24351</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1559110</v>
+      </c>
+      <c r="B6" s="7">
+        <v>45519</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>3.2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>24350</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>45519</v>
+      </c>
+      <c r="C7">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>3.2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>24358</v>
+      </c>
+      <c r="J7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NTN&amp;2311</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>550</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>ROTA ITINERANTE DE 2 DIAS</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1559111</v>
+      </c>
+      <c r="B8" s="7">
+        <v>45519</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>4.09</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>215874</v>
+      <c r="H8">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>24352</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajustado quando nao acha o manifesto
</commit_message>
<xml_diff>
--- a/EVENTO.xlsx
+++ b/EVENTO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jetta\Documents\Efetuar_Evento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\Efetuar_Evento\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC0A438-D7C3-4EFF-925C-14A6B70F0069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="19170" windowHeight="11400"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>EVENTO</t>
   </si>
@@ -50,9 +51,6 @@
   </si>
   <si>
     <t>MOTIVO</t>
-  </si>
-  <si>
-    <t>ESU-5H70</t>
   </si>
   <si>
     <t>REEMBOLSO DE PEDAGIO</t>
@@ -91,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,7 +204,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,19 +517,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -568,36 +565,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1559341</v>
-      </c>
-      <c r="B2" s="7">
-        <v>45517</v>
-      </c>
-      <c r="C2">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>122.42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>215905</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
@@ -896,7 +864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -948,13 +916,13 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>76.2</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -977,13 +945,13 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>22.8</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1006,13 +974,13 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>10.3</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1024,7 +992,7 @@
         <v>24362</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1035,13 +1003,13 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>3.2</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1053,7 +1021,7 @@
         <v>24351</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1067,13 +1035,13 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>3.2</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1085,7 +1053,7 @@
         <v>24350</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1096,13 +1064,13 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>3.2</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1114,7 +1082,7 @@
         <v>24358</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1128,13 +1096,13 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>4.09</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1146,7 +1114,7 @@
         <v>24352</v>
       </c>
       <c r="J8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>